<commit_message>
added original planned pit locations, used these to add coordinates to missing pit xlxs files, added more notes to CODE/README.md
</commit_message>
<xml_diff>
--- a/PITS/B01_Pit_26Mar2019.xlsx
+++ b/PITS/B01_Pit_26Mar2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpm/HP_DRIVE/GrandMesaMarch2019/PITS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC640CE-7582-8A4E-804D-50192F174489}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC87EF-5377-3E43-AD5A-34AE8A5681FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="29920" windowHeight="17820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,13 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">ENVIRONMENT!$A$1:$R$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">PIT!$B$1:$AF$33</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1221,7 +1226,8 @@
   <si>
     <t>SMP 35-38
 4 Density measurements @ 19-9
-325 measurement had grass</t>
+325 measurement had grass
+Coordinates added from planned location.</t>
   </si>
 </sst>
 </file>
@@ -3540,11 +3546,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -3609,9 +3624,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="124" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -3663,6 +3675,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3753,21 +3771,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3810,7 +3813,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3828,12 +3834,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3852,6 +3852,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3871,6 +3874,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="117" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4841,7 +4847,7 @@
   <dimension ref="A1:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14:AF15"/>
+      <selection activeCell="L2" sqref="L2:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -4905,18 +4911,18 @@
       <c r="T1" s="316"/>
       <c r="U1" s="316"/>
       <c r="V1" s="317"/>
-      <c r="W1" s="214" t="s">
+      <c r="W1" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="215"/>
-      <c r="Y1" s="215"/>
-      <c r="Z1" s="215"/>
-      <c r="AA1" s="215"/>
-      <c r="AB1" s="215"/>
-      <c r="AC1" s="215"/>
-      <c r="AD1" s="215"/>
-      <c r="AE1" s="215"/>
-      <c r="AF1" s="216"/>
+      <c r="X1" s="217"/>
+      <c r="Y1" s="217"/>
+      <c r="Z1" s="217"/>
+      <c r="AA1" s="217"/>
+      <c r="AB1" s="217"/>
+      <c r="AC1" s="217"/>
+      <c r="AD1" s="217"/>
+      <c r="AE1" s="217"/>
+      <c r="AF1" s="218"/>
     </row>
     <row r="2" spans="1:32" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="24"/>
@@ -4945,35 +4951,35 @@
       <c r="T2" s="319"/>
       <c r="U2" s="319"/>
       <c r="V2" s="320"/>
-      <c r="W2" s="217" t="s">
+      <c r="W2" s="219" t="s">
         <v>303</v>
       </c>
-      <c r="X2" s="218"/>
-      <c r="Y2" s="218"/>
-      <c r="Z2" s="218"/>
-      <c r="AA2" s="218"/>
-      <c r="AB2" s="218"/>
-      <c r="AC2" s="218"/>
-      <c r="AD2" s="218"/>
-      <c r="AE2" s="218"/>
-      <c r="AF2" s="219"/>
+      <c r="X2" s="220"/>
+      <c r="Y2" s="220"/>
+      <c r="Z2" s="220"/>
+      <c r="AA2" s="220"/>
+      <c r="AB2" s="220"/>
+      <c r="AC2" s="220"/>
+      <c r="AD2" s="220"/>
+      <c r="AE2" s="220"/>
+      <c r="AF2" s="221"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="201"/>
-      <c r="G3" s="201"/>
-      <c r="H3" s="201"/>
-      <c r="I3" s="204" t="s">
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="207" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="205"/>
-      <c r="K3" s="206"/>
+      <c r="J3" s="208"/>
+      <c r="K3" s="209"/>
       <c r="L3" s="323" t="s">
         <v>5</v>
       </c>
@@ -4983,77 +4989,81 @@
       <c r="P3" s="321" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="201"/>
-      <c r="R3" s="201"/>
-      <c r="S3" s="201"/>
-      <c r="T3" s="201"/>
+      <c r="Q3" s="204"/>
+      <c r="R3" s="204"/>
+      <c r="S3" s="204"/>
+      <c r="T3" s="204"/>
       <c r="U3" s="322"/>
       <c r="V3" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="220"/>
-      <c r="X3" s="221"/>
-      <c r="Y3" s="221"/>
-      <c r="Z3" s="221"/>
-      <c r="AA3" s="221"/>
-      <c r="AB3" s="221"/>
-      <c r="AC3" s="221"/>
-      <c r="AD3" s="221"/>
-      <c r="AE3" s="221"/>
-      <c r="AF3" s="222"/>
+      <c r="W3" s="222"/>
+      <c r="X3" s="223"/>
+      <c r="Y3" s="223"/>
+      <c r="Z3" s="223"/>
+      <c r="AA3" s="223"/>
+      <c r="AB3" s="223"/>
+      <c r="AC3" s="223"/>
+      <c r="AD3" s="223"/>
+      <c r="AE3" s="223"/>
+      <c r="AF3" s="224"/>
     </row>
     <row r="4" spans="1:32" ht="29" customHeight="1" thickBot="1">
       <c r="A4" s="24"/>
-      <c r="B4" s="202"/>
-      <c r="C4" s="203"/>
-      <c r="D4" s="203"/>
-      <c r="E4" s="203"/>
-      <c r="F4" s="203"/>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="207"/>
-      <c r="J4" s="208"/>
-      <c r="K4" s="208"/>
-      <c r="L4" s="327"/>
+      <c r="B4" s="205"/>
+      <c r="C4" s="206"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="206"/>
+      <c r="F4" s="206"/>
+      <c r="G4" s="206"/>
+      <c r="H4" s="206"/>
+      <c r="I4" s="210"/>
+      <c r="J4" s="211"/>
+      <c r="K4" s="211"/>
+      <c r="L4" s="327">
+        <v>741267</v>
+      </c>
       <c r="M4" s="328"/>
       <c r="N4" s="328"/>
       <c r="O4" s="329"/>
-      <c r="P4" s="328"/>
+      <c r="P4" s="328">
+        <v>4322950</v>
+      </c>
       <c r="Q4" s="328"/>
       <c r="R4" s="328"/>
       <c r="S4" s="328"/>
       <c r="T4" s="328"/>
       <c r="U4" s="329"/>
       <c r="V4" s="169"/>
-      <c r="W4" s="220"/>
-      <c r="X4" s="221"/>
-      <c r="Y4" s="221"/>
-      <c r="Z4" s="221"/>
-      <c r="AA4" s="221"/>
-      <c r="AB4" s="221"/>
-      <c r="AC4" s="221"/>
-      <c r="AD4" s="221"/>
-      <c r="AE4" s="221"/>
-      <c r="AF4" s="222"/>
+      <c r="W4" s="222"/>
+      <c r="X4" s="223"/>
+      <c r="Y4" s="223"/>
+      <c r="Z4" s="223"/>
+      <c r="AA4" s="223"/>
+      <c r="AB4" s="223"/>
+      <c r="AC4" s="223"/>
+      <c r="AD4" s="223"/>
+      <c r="AE4" s="223"/>
+      <c r="AF4" s="224"/>
     </row>
     <row r="5" spans="1:32" ht="29" customHeight="1">
       <c r="A5" s="24"/>
-      <c r="B5" s="226" t="s">
+      <c r="B5" s="228" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="209" t="s">
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="212" t="s">
         <v>192</v>
       </c>
-      <c r="H5" s="210"/>
-      <c r="I5" s="198" t="s">
+      <c r="H5" s="213"/>
+      <c r="I5" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="J5" s="198"/>
-      <c r="K5" s="199"/>
+      <c r="J5" s="201"/>
+      <c r="K5" s="202"/>
       <c r="L5" s="330" t="s">
         <v>255</v>
       </c>
@@ -5062,43 +5072,43 @@
         <v>8</v>
       </c>
       <c r="O5" s="333"/>
-      <c r="P5" s="190" t="s">
+      <c r="P5" s="193" t="s">
         <v>169</v>
       </c>
-      <c r="Q5" s="191"/>
-      <c r="R5" s="194" t="s">
+      <c r="Q5" s="194"/>
+      <c r="R5" s="197" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="194"/>
-      <c r="T5" s="194"/>
-      <c r="U5" s="191"/>
+      <c r="S5" s="197"/>
+      <c r="T5" s="197"/>
+      <c r="U5" s="194"/>
       <c r="V5" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="220"/>
-      <c r="X5" s="221"/>
-      <c r="Y5" s="221"/>
-      <c r="Z5" s="221"/>
-      <c r="AA5" s="221"/>
-      <c r="AB5" s="221"/>
-      <c r="AC5" s="221"/>
-      <c r="AD5" s="221"/>
-      <c r="AE5" s="221"/>
-      <c r="AF5" s="222"/>
+      <c r="W5" s="222"/>
+      <c r="X5" s="223"/>
+      <c r="Y5" s="223"/>
+      <c r="Z5" s="223"/>
+      <c r="AA5" s="223"/>
+      <c r="AB5" s="223"/>
+      <c r="AC5" s="223"/>
+      <c r="AD5" s="223"/>
+      <c r="AE5" s="223"/>
+      <c r="AF5" s="224"/>
     </row>
     <row r="6" spans="1:32" ht="32" customHeight="1" thickBot="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="228" t="s">
+      <c r="B6" s="230" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="229"/>
-      <c r="D6" s="229"/>
-      <c r="E6" s="229"/>
-      <c r="F6" s="229"/>
-      <c r="G6" s="211">
+      <c r="C6" s="231"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="231"/>
+      <c r="F6" s="231"/>
+      <c r="G6" s="214">
         <v>139</v>
       </c>
-      <c r="H6" s="212"/>
+      <c r="H6" s="215"/>
       <c r="I6" s="176" t="s">
         <v>268</v>
       </c>
@@ -5117,30 +5127,30 @@
       <c r="N6" s="334">
         <v>0</v>
       </c>
-      <c r="O6" s="193"/>
-      <c r="P6" s="192" t="s">
+      <c r="O6" s="196"/>
+      <c r="P6" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="193"/>
-      <c r="R6" s="195">
+      <c r="Q6" s="196"/>
+      <c r="R6" s="198">
         <v>43550</v>
       </c>
-      <c r="S6" s="196"/>
-      <c r="T6" s="196"/>
-      <c r="U6" s="197"/>
+      <c r="S6" s="199"/>
+      <c r="T6" s="199"/>
+      <c r="U6" s="200"/>
       <c r="V6" s="45">
         <v>1358</v>
       </c>
-      <c r="W6" s="223"/>
-      <c r="X6" s="224"/>
-      <c r="Y6" s="224"/>
-      <c r="Z6" s="224"/>
-      <c r="AA6" s="224"/>
-      <c r="AB6" s="224"/>
-      <c r="AC6" s="224"/>
-      <c r="AD6" s="224"/>
-      <c r="AE6" s="224"/>
-      <c r="AF6" s="225"/>
+      <c r="W6" s="225"/>
+      <c r="X6" s="226"/>
+      <c r="Y6" s="226"/>
+      <c r="Z6" s="226"/>
+      <c r="AA6" s="226"/>
+      <c r="AB6" s="226"/>
+      <c r="AC6" s="226"/>
+      <c r="AD6" s="226"/>
+      <c r="AE6" s="226"/>
+      <c r="AF6" s="227"/>
     </row>
     <row r="7" spans="1:32" s="6" customFormat="1" ht="29" customHeight="1">
       <c r="A7" s="25"/>
@@ -5152,37 +5162,37 @@
       <c r="E7" s="309"/>
       <c r="F7" s="309"/>
       <c r="G7" s="310"/>
-      <c r="H7" s="244" t="s">
+      <c r="H7" s="248" t="s">
         <v>97</v>
       </c>
-      <c r="I7" s="245"/>
-      <c r="J7" s="245"/>
-      <c r="K7" s="246"/>
-      <c r="L7" s="242" t="s">
+      <c r="I7" s="249"/>
+      <c r="J7" s="249"/>
+      <c r="K7" s="250"/>
+      <c r="L7" s="246" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="243"/>
-      <c r="N7" s="239"/>
-      <c r="O7" s="236" t="s">
+      <c r="M7" s="247"/>
+      <c r="N7" s="243"/>
+      <c r="O7" s="240" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="237"/>
-      <c r="Q7" s="237"/>
-      <c r="R7" s="237"/>
-      <c r="S7" s="237"/>
-      <c r="T7" s="237"/>
-      <c r="U7" s="237"/>
-      <c r="V7" s="237"/>
-      <c r="W7" s="237"/>
-      <c r="X7" s="237"/>
-      <c r="Y7" s="237"/>
-      <c r="Z7" s="237"/>
-      <c r="AA7" s="237"/>
-      <c r="AB7" s="237"/>
-      <c r="AC7" s="237"/>
-      <c r="AD7" s="237"/>
-      <c r="AE7" s="237"/>
-      <c r="AF7" s="238"/>
+      <c r="P7" s="241"/>
+      <c r="Q7" s="241"/>
+      <c r="R7" s="241"/>
+      <c r="S7" s="241"/>
+      <c r="T7" s="241"/>
+      <c r="U7" s="241"/>
+      <c r="V7" s="241"/>
+      <c r="W7" s="241"/>
+      <c r="X7" s="241"/>
+      <c r="Y7" s="241"/>
+      <c r="Z7" s="241"/>
+      <c r="AA7" s="241"/>
+      <c r="AB7" s="241"/>
+      <c r="AC7" s="241"/>
+      <c r="AD7" s="241"/>
+      <c r="AE7" s="241"/>
+      <c r="AF7" s="242"/>
     </row>
     <row r="8" spans="1:32" ht="37.25" customHeight="1">
       <c r="B8" s="313" t="s">
@@ -5213,37 +5223,37 @@
       <c r="M8" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="240"/>
-      <c r="O8" s="265" t="s">
+      <c r="N8" s="244"/>
+      <c r="O8" s="264" t="s">
         <v>87</v>
       </c>
-      <c r="P8" s="266"/>
-      <c r="Q8" s="234"/>
-      <c r="R8" s="267" t="s">
+      <c r="P8" s="265"/>
+      <c r="Q8" s="238"/>
+      <c r="R8" s="266" t="s">
         <v>105</v>
       </c>
-      <c r="S8" s="268"/>
-      <c r="T8" s="269"/>
+      <c r="S8" s="267"/>
+      <c r="T8" s="268"/>
       <c r="U8" s="314" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="234" t="s">
+      <c r="V8" s="238" t="s">
         <v>53</v>
       </c>
-      <c r="W8" s="232" t="s">
+      <c r="W8" s="236" t="s">
         <v>108</v>
       </c>
-      <c r="X8" s="247" t="s">
+      <c r="X8" s="251" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" s="247"/>
-      <c r="Z8" s="247"/>
-      <c r="AA8" s="247"/>
-      <c r="AB8" s="247"/>
-      <c r="AC8" s="247"/>
-      <c r="AD8" s="247"/>
-      <c r="AE8" s="247"/>
-      <c r="AF8" s="248"/>
+      <c r="Y8" s="251"/>
+      <c r="Z8" s="251"/>
+      <c r="AA8" s="251"/>
+      <c r="AB8" s="251"/>
+      <c r="AC8" s="251"/>
+      <c r="AD8" s="251"/>
+      <c r="AE8" s="251"/>
+      <c r="AF8" s="252"/>
     </row>
     <row r="9" spans="1:32" ht="29" customHeight="1">
       <c r="B9" s="29" t="s">
@@ -5282,7 +5292,7 @@
       <c r="M9" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="N9" s="240"/>
+      <c r="N9" s="244"/>
       <c r="O9" s="104" t="s">
         <v>19</v>
       </c>
@@ -5302,17 +5312,17 @@
         <v>207</v>
       </c>
       <c r="U9" s="314"/>
-      <c r="V9" s="235"/>
-      <c r="W9" s="233"/>
-      <c r="X9" s="249"/>
-      <c r="Y9" s="249"/>
-      <c r="Z9" s="249"/>
-      <c r="AA9" s="249"/>
-      <c r="AB9" s="249"/>
-      <c r="AC9" s="249"/>
-      <c r="AD9" s="249"/>
-      <c r="AE9" s="249"/>
-      <c r="AF9" s="250"/>
+      <c r="V9" s="239"/>
+      <c r="W9" s="237"/>
+      <c r="X9" s="253"/>
+      <c r="Y9" s="253"/>
+      <c r="Z9" s="253"/>
+      <c r="AA9" s="253"/>
+      <c r="AB9" s="253"/>
+      <c r="AC9" s="253"/>
+      <c r="AD9" s="253"/>
+      <c r="AE9" s="253"/>
+      <c r="AF9" s="254"/>
     </row>
     <row r="10" spans="1:32" ht="20" customHeight="1">
       <c r="B10" s="9" t="s">
@@ -5331,37 +5341,37 @@
       <c r="K10" s="10"/>
       <c r="L10" s="70"/>
       <c r="M10" s="66"/>
-      <c r="N10" s="240"/>
+      <c r="N10" s="244"/>
       <c r="O10" s="326">
         <v>139</v>
       </c>
-      <c r="P10" s="264" t="s">
+      <c r="P10" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="264" t="s">
+      <c r="Q10" s="192" t="s">
         <v>292</v>
       </c>
-      <c r="R10" s="286"/>
-      <c r="S10" s="262" t="s">
+      <c r="R10" s="279"/>
+      <c r="S10" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="T10" s="270"/>
-      <c r="U10" s="285" t="s">
+      <c r="T10" s="269"/>
+      <c r="U10" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V10" s="260" t="s">
+      <c r="V10" s="188" t="s">
         <v>63</v>
       </c>
-      <c r="W10" s="230"/>
-      <c r="X10" s="275"/>
-      <c r="Y10" s="251"/>
-      <c r="Z10" s="251"/>
-      <c r="AA10" s="251"/>
-      <c r="AB10" s="251"/>
-      <c r="AC10" s="251"/>
-      <c r="AD10" s="251"/>
-      <c r="AE10" s="251"/>
-      <c r="AF10" s="252"/>
+      <c r="W10" s="234"/>
+      <c r="X10" s="274"/>
+      <c r="Y10" s="255"/>
+      <c r="Z10" s="255"/>
+      <c r="AA10" s="255"/>
+      <c r="AB10" s="255"/>
+      <c r="AC10" s="255"/>
+      <c r="AD10" s="255"/>
+      <c r="AE10" s="255"/>
+      <c r="AF10" s="256"/>
     </row>
     <row r="11" spans="1:32" ht="20" customHeight="1">
       <c r="B11" s="9">
@@ -5390,25 +5400,25 @@
       <c r="M11" s="64">
         <v>-1.6</v>
       </c>
-      <c r="N11" s="240"/>
-      <c r="O11" s="261"/>
-      <c r="P11" s="264"/>
-      <c r="Q11" s="264"/>
-      <c r="R11" s="262"/>
-      <c r="S11" s="262"/>
-      <c r="T11" s="271"/>
-      <c r="U11" s="286"/>
-      <c r="V11" s="277"/>
-      <c r="W11" s="231"/>
-      <c r="X11" s="276"/>
-      <c r="Y11" s="255"/>
-      <c r="Z11" s="255"/>
-      <c r="AA11" s="255"/>
-      <c r="AB11" s="255"/>
-      <c r="AC11" s="255"/>
-      <c r="AD11" s="255"/>
-      <c r="AE11" s="255"/>
-      <c r="AF11" s="256"/>
+      <c r="N11" s="244"/>
+      <c r="O11" s="189"/>
+      <c r="P11" s="192"/>
+      <c r="Q11" s="192"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="270"/>
+      <c r="U11" s="279"/>
+      <c r="V11" s="276"/>
+      <c r="W11" s="235"/>
+      <c r="X11" s="275"/>
+      <c r="Y11" s="259"/>
+      <c r="Z11" s="259"/>
+      <c r="AA11" s="259"/>
+      <c r="AB11" s="259"/>
+      <c r="AC11" s="259"/>
+      <c r="AD11" s="259"/>
+      <c r="AE11" s="259"/>
+      <c r="AF11" s="260"/>
     </row>
     <row r="12" spans="1:32" ht="20" customHeight="1">
       <c r="B12" s="9">
@@ -5439,38 +5449,38 @@
       <c r="M12" s="62">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="N12" s="240"/>
-      <c r="O12" s="260" t="str">
+      <c r="N12" s="244"/>
+      <c r="O12" s="188" t="str">
         <f>Q10</f>
         <v>136</v>
       </c>
-      <c r="P12" s="264" t="s">
+      <c r="P12" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="264" t="s">
+      <c r="Q12" s="192" t="s">
         <v>293</v>
       </c>
-      <c r="R12" s="262" t="s">
+      <c r="R12" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="S12" s="262"/>
-      <c r="T12" s="278"/>
-      <c r="U12" s="285" t="s">
+      <c r="S12" s="190"/>
+      <c r="T12" s="277"/>
+      <c r="U12" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V12" s="260" t="s">
+      <c r="V12" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="W12" s="188"/>
-      <c r="X12" s="251"/>
-      <c r="Y12" s="251"/>
-      <c r="Z12" s="251"/>
-      <c r="AA12" s="251"/>
-      <c r="AB12" s="251"/>
-      <c r="AC12" s="251"/>
-      <c r="AD12" s="251"/>
-      <c r="AE12" s="251"/>
-      <c r="AF12" s="252"/>
+      <c r="W12" s="232"/>
+      <c r="X12" s="255"/>
+      <c r="Y12" s="255"/>
+      <c r="Z12" s="255"/>
+      <c r="AA12" s="255"/>
+      <c r="AB12" s="255"/>
+      <c r="AC12" s="255"/>
+      <c r="AD12" s="255"/>
+      <c r="AE12" s="255"/>
+      <c r="AF12" s="256"/>
     </row>
     <row r="13" spans="1:32" ht="20" customHeight="1">
       <c r="B13" s="9">
@@ -5501,25 +5511,25 @@
       <c r="M13" s="66">
         <v>-4.4000000000000004</v>
       </c>
-      <c r="N13" s="240"/>
-      <c r="O13" s="261"/>
-      <c r="P13" s="264"/>
-      <c r="Q13" s="264"/>
-      <c r="R13" s="262"/>
-      <c r="S13" s="262"/>
-      <c r="T13" s="278"/>
-      <c r="U13" s="286"/>
-      <c r="V13" s="277"/>
-      <c r="W13" s="189"/>
-      <c r="X13" s="255"/>
-      <c r="Y13" s="255"/>
-      <c r="Z13" s="255"/>
-      <c r="AA13" s="255"/>
-      <c r="AB13" s="255"/>
-      <c r="AC13" s="255"/>
-      <c r="AD13" s="255"/>
-      <c r="AE13" s="255"/>
-      <c r="AF13" s="256"/>
+      <c r="N13" s="244"/>
+      <c r="O13" s="189"/>
+      <c r="P13" s="192"/>
+      <c r="Q13" s="192"/>
+      <c r="R13" s="190"/>
+      <c r="S13" s="190"/>
+      <c r="T13" s="277"/>
+      <c r="U13" s="279"/>
+      <c r="V13" s="276"/>
+      <c r="W13" s="233"/>
+      <c r="X13" s="259"/>
+      <c r="Y13" s="259"/>
+      <c r="Z13" s="259"/>
+      <c r="AA13" s="259"/>
+      <c r="AB13" s="259"/>
+      <c r="AC13" s="259"/>
+      <c r="AD13" s="259"/>
+      <c r="AE13" s="259"/>
+      <c r="AF13" s="260"/>
     </row>
     <row r="14" spans="1:32" ht="20" customHeight="1">
       <c r="B14" s="9">
@@ -5550,38 +5560,38 @@
       <c r="M14" s="66">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="N14" s="240"/>
-      <c r="O14" s="260" t="str">
+      <c r="N14" s="244"/>
+      <c r="O14" s="188" t="str">
         <f t="shared" ref="O14" si="2">Q12</f>
         <v>133</v>
       </c>
-      <c r="P14" s="264" t="s">
+      <c r="P14" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q14" s="264" t="s">
+      <c r="Q14" s="192" t="s">
         <v>294</v>
       </c>
-      <c r="R14" s="262" t="s">
+      <c r="R14" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="S14" s="263"/>
-      <c r="T14" s="272"/>
-      <c r="U14" s="285" t="s">
+      <c r="S14" s="191"/>
+      <c r="T14" s="271"/>
+      <c r="U14" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V14" s="260" t="s">
+      <c r="V14" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="W14" s="188"/>
-      <c r="X14" s="251"/>
-      <c r="Y14" s="251"/>
-      <c r="Z14" s="251"/>
-      <c r="AA14" s="251"/>
-      <c r="AB14" s="251"/>
-      <c r="AC14" s="251"/>
-      <c r="AD14" s="251"/>
-      <c r="AE14" s="251"/>
-      <c r="AF14" s="252"/>
+      <c r="W14" s="232"/>
+      <c r="X14" s="255"/>
+      <c r="Y14" s="255"/>
+      <c r="Z14" s="255"/>
+      <c r="AA14" s="255"/>
+      <c r="AB14" s="255"/>
+      <c r="AC14" s="255"/>
+      <c r="AD14" s="255"/>
+      <c r="AE14" s="255"/>
+      <c r="AF14" s="256"/>
     </row>
     <row r="15" spans="1:32" ht="20" customHeight="1">
       <c r="B15" s="9">
@@ -5612,25 +5622,25 @@
       <c r="M15" s="63">
         <v>-3.5</v>
       </c>
-      <c r="N15" s="240"/>
-      <c r="O15" s="261"/>
-      <c r="P15" s="264"/>
-      <c r="Q15" s="264"/>
-      <c r="R15" s="262"/>
-      <c r="S15" s="263"/>
-      <c r="T15" s="274"/>
-      <c r="U15" s="286"/>
-      <c r="V15" s="277"/>
-      <c r="W15" s="189"/>
-      <c r="X15" s="255"/>
-      <c r="Y15" s="255"/>
-      <c r="Z15" s="255"/>
-      <c r="AA15" s="255"/>
-      <c r="AB15" s="255"/>
-      <c r="AC15" s="255"/>
-      <c r="AD15" s="255"/>
-      <c r="AE15" s="255"/>
-      <c r="AF15" s="256"/>
+      <c r="N15" s="244"/>
+      <c r="O15" s="189"/>
+      <c r="P15" s="192"/>
+      <c r="Q15" s="192"/>
+      <c r="R15" s="190"/>
+      <c r="S15" s="191"/>
+      <c r="T15" s="273"/>
+      <c r="U15" s="279"/>
+      <c r="V15" s="276"/>
+      <c r="W15" s="233"/>
+      <c r="X15" s="259"/>
+      <c r="Y15" s="259"/>
+      <c r="Z15" s="259"/>
+      <c r="AA15" s="259"/>
+      <c r="AB15" s="259"/>
+      <c r="AC15" s="259"/>
+      <c r="AD15" s="259"/>
+      <c r="AE15" s="259"/>
+      <c r="AF15" s="260"/>
     </row>
     <row r="16" spans="1:32" ht="20" customHeight="1">
       <c r="B16" s="9">
@@ -5661,38 +5671,38 @@
       <c r="M16" s="66">
         <v>-3.4</v>
       </c>
-      <c r="N16" s="240"/>
-      <c r="O16" s="260" t="str">
+      <c r="N16" s="244"/>
+      <c r="O16" s="188" t="str">
         <f t="shared" ref="O16" si="3">Q14</f>
         <v>117</v>
       </c>
-      <c r="P16" s="264" t="s">
+      <c r="P16" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q16" s="264" t="s">
+      <c r="Q16" s="192" t="s">
         <v>295</v>
       </c>
-      <c r="R16" s="262" t="s">
+      <c r="R16" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="S16" s="263"/>
-      <c r="T16" s="272"/>
-      <c r="U16" s="285" t="s">
+      <c r="S16" s="191"/>
+      <c r="T16" s="271"/>
+      <c r="U16" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V16" s="260" t="s">
+      <c r="V16" s="188" t="s">
         <v>63</v>
       </c>
-      <c r="W16" s="188"/>
-      <c r="X16" s="251"/>
-      <c r="Y16" s="251"/>
-      <c r="Z16" s="251"/>
-      <c r="AA16" s="251"/>
-      <c r="AB16" s="251"/>
-      <c r="AC16" s="251"/>
-      <c r="AD16" s="251"/>
-      <c r="AE16" s="251"/>
-      <c r="AF16" s="252"/>
+      <c r="W16" s="232"/>
+      <c r="X16" s="255"/>
+      <c r="Y16" s="255"/>
+      <c r="Z16" s="255"/>
+      <c r="AA16" s="255"/>
+      <c r="AB16" s="255"/>
+      <c r="AC16" s="255"/>
+      <c r="AD16" s="255"/>
+      <c r="AE16" s="255"/>
+      <c r="AF16" s="256"/>
     </row>
     <row r="17" spans="2:32" ht="20" customHeight="1">
       <c r="B17" s="9">
@@ -5725,25 +5735,25 @@
       <c r="M17" s="63">
         <v>-3.1</v>
       </c>
-      <c r="N17" s="240"/>
-      <c r="O17" s="261"/>
-      <c r="P17" s="264"/>
-      <c r="Q17" s="264"/>
-      <c r="R17" s="262"/>
-      <c r="S17" s="263"/>
-      <c r="T17" s="273"/>
-      <c r="U17" s="286"/>
-      <c r="V17" s="277"/>
-      <c r="W17" s="189"/>
-      <c r="X17" s="255"/>
-      <c r="Y17" s="255"/>
-      <c r="Z17" s="255"/>
-      <c r="AA17" s="255"/>
-      <c r="AB17" s="255"/>
-      <c r="AC17" s="255"/>
-      <c r="AD17" s="255"/>
-      <c r="AE17" s="255"/>
-      <c r="AF17" s="256"/>
+      <c r="N17" s="244"/>
+      <c r="O17" s="189"/>
+      <c r="P17" s="192"/>
+      <c r="Q17" s="192"/>
+      <c r="R17" s="190"/>
+      <c r="S17" s="191"/>
+      <c r="T17" s="272"/>
+      <c r="U17" s="279"/>
+      <c r="V17" s="276"/>
+      <c r="W17" s="233"/>
+      <c r="X17" s="259"/>
+      <c r="Y17" s="259"/>
+      <c r="Z17" s="259"/>
+      <c r="AA17" s="259"/>
+      <c r="AB17" s="259"/>
+      <c r="AC17" s="259"/>
+      <c r="AD17" s="259"/>
+      <c r="AE17" s="259"/>
+      <c r="AF17" s="260"/>
     </row>
     <row r="18" spans="2:32" ht="20" customHeight="1">
       <c r="B18" s="9">
@@ -5774,38 +5784,38 @@
       <c r="M18" s="67">
         <v>-2.8</v>
       </c>
-      <c r="N18" s="240"/>
-      <c r="O18" s="260" t="str">
+      <c r="N18" s="244"/>
+      <c r="O18" s="188" t="str">
         <f t="shared" ref="O18" si="4">Q16</f>
         <v>98</v>
       </c>
-      <c r="P18" s="264" t="s">
+      <c r="P18" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q18" s="264" t="s">
+      <c r="Q18" s="192" t="s">
         <v>296</v>
       </c>
-      <c r="R18" s="262" t="s">
+      <c r="R18" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="S18" s="263"/>
-      <c r="T18" s="274"/>
-      <c r="U18" s="285" t="s">
+      <c r="S18" s="191"/>
+      <c r="T18" s="273"/>
+      <c r="U18" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V18" s="260" t="s">
+      <c r="V18" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="W18" s="188"/>
-      <c r="X18" s="251"/>
-      <c r="Y18" s="251"/>
-      <c r="Z18" s="251"/>
-      <c r="AA18" s="251"/>
-      <c r="AB18" s="251"/>
-      <c r="AC18" s="251"/>
-      <c r="AD18" s="251"/>
-      <c r="AE18" s="251"/>
-      <c r="AF18" s="252"/>
+      <c r="W18" s="232"/>
+      <c r="X18" s="255"/>
+      <c r="Y18" s="255"/>
+      <c r="Z18" s="255"/>
+      <c r="AA18" s="255"/>
+      <c r="AB18" s="255"/>
+      <c r="AC18" s="255"/>
+      <c r="AD18" s="255"/>
+      <c r="AE18" s="255"/>
+      <c r="AF18" s="256"/>
     </row>
     <row r="19" spans="2:32" ht="20" customHeight="1">
       <c r="B19" s="9">
@@ -5836,25 +5846,25 @@
       <c r="M19" s="63">
         <v>-2.4</v>
       </c>
-      <c r="N19" s="240"/>
-      <c r="O19" s="261"/>
-      <c r="P19" s="264"/>
-      <c r="Q19" s="264"/>
-      <c r="R19" s="262"/>
-      <c r="S19" s="263"/>
-      <c r="T19" s="273"/>
-      <c r="U19" s="286"/>
-      <c r="V19" s="277"/>
-      <c r="W19" s="189"/>
-      <c r="X19" s="255"/>
-      <c r="Y19" s="255"/>
-      <c r="Z19" s="255"/>
-      <c r="AA19" s="255"/>
-      <c r="AB19" s="255"/>
-      <c r="AC19" s="255"/>
-      <c r="AD19" s="255"/>
-      <c r="AE19" s="255"/>
-      <c r="AF19" s="256"/>
+      <c r="N19" s="244"/>
+      <c r="O19" s="189"/>
+      <c r="P19" s="192"/>
+      <c r="Q19" s="192"/>
+      <c r="R19" s="190"/>
+      <c r="S19" s="191"/>
+      <c r="T19" s="272"/>
+      <c r="U19" s="279"/>
+      <c r="V19" s="276"/>
+      <c r="W19" s="233"/>
+      <c r="X19" s="259"/>
+      <c r="Y19" s="259"/>
+      <c r="Z19" s="259"/>
+      <c r="AA19" s="259"/>
+      <c r="AB19" s="259"/>
+      <c r="AC19" s="259"/>
+      <c r="AD19" s="259"/>
+      <c r="AE19" s="259"/>
+      <c r="AF19" s="260"/>
     </row>
     <row r="20" spans="2:32" ht="20" customHeight="1">
       <c r="B20" s="9">
@@ -5885,38 +5895,38 @@
       <c r="M20" s="67">
         <v>-2.1</v>
       </c>
-      <c r="N20" s="240"/>
-      <c r="O20" s="260" t="str">
+      <c r="N20" s="244"/>
+      <c r="O20" s="188" t="str">
         <f t="shared" ref="O20" si="5">Q18</f>
         <v>87</v>
       </c>
-      <c r="P20" s="264" t="s">
+      <c r="P20" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q20" s="264" t="s">
+      <c r="Q20" s="192" t="s">
         <v>297</v>
       </c>
-      <c r="R20" s="262" t="s">
+      <c r="R20" s="190" t="s">
         <v>301</v>
       </c>
-      <c r="S20" s="263"/>
-      <c r="T20" s="274"/>
-      <c r="U20" s="285" t="s">
+      <c r="S20" s="191"/>
+      <c r="T20" s="273"/>
+      <c r="U20" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V20" s="260" t="s">
+      <c r="V20" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="W20" s="188"/>
-      <c r="X20" s="251"/>
-      <c r="Y20" s="251"/>
-      <c r="Z20" s="251"/>
-      <c r="AA20" s="251"/>
-      <c r="AB20" s="251"/>
-      <c r="AC20" s="251"/>
-      <c r="AD20" s="251"/>
-      <c r="AE20" s="251"/>
-      <c r="AF20" s="252"/>
+      <c r="W20" s="232"/>
+      <c r="X20" s="255"/>
+      <c r="Y20" s="255"/>
+      <c r="Z20" s="255"/>
+      <c r="AA20" s="255"/>
+      <c r="AB20" s="255"/>
+      <c r="AC20" s="255"/>
+      <c r="AD20" s="255"/>
+      <c r="AE20" s="255"/>
+      <c r="AF20" s="256"/>
     </row>
     <row r="21" spans="2:32" ht="20" customHeight="1">
       <c r="B21" s="9">
@@ -5947,25 +5957,25 @@
       <c r="M21" s="63">
         <v>-1.3</v>
       </c>
-      <c r="N21" s="240"/>
-      <c r="O21" s="261"/>
-      <c r="P21" s="264"/>
-      <c r="Q21" s="264"/>
-      <c r="R21" s="262"/>
-      <c r="S21" s="263"/>
-      <c r="T21" s="273"/>
-      <c r="U21" s="286"/>
-      <c r="V21" s="277"/>
-      <c r="W21" s="189"/>
-      <c r="X21" s="255"/>
-      <c r="Y21" s="255"/>
-      <c r="Z21" s="255"/>
-      <c r="AA21" s="255"/>
-      <c r="AB21" s="255"/>
-      <c r="AC21" s="255"/>
-      <c r="AD21" s="255"/>
-      <c r="AE21" s="255"/>
-      <c r="AF21" s="256"/>
+      <c r="N21" s="244"/>
+      <c r="O21" s="189"/>
+      <c r="P21" s="192"/>
+      <c r="Q21" s="192"/>
+      <c r="R21" s="190"/>
+      <c r="S21" s="191"/>
+      <c r="T21" s="272"/>
+      <c r="U21" s="279"/>
+      <c r="V21" s="276"/>
+      <c r="W21" s="233"/>
+      <c r="X21" s="259"/>
+      <c r="Y21" s="259"/>
+      <c r="Z21" s="259"/>
+      <c r="AA21" s="259"/>
+      <c r="AB21" s="259"/>
+      <c r="AC21" s="259"/>
+      <c r="AD21" s="259"/>
+      <c r="AE21" s="259"/>
+      <c r="AF21" s="260"/>
     </row>
     <row r="22" spans="2:32" ht="20" customHeight="1">
       <c r="B22" s="9">
@@ -5996,38 +6006,38 @@
       <c r="M22" s="67">
         <v>-0.8</v>
       </c>
-      <c r="N22" s="240"/>
-      <c r="O22" s="260" t="str">
+      <c r="N22" s="244"/>
+      <c r="O22" s="188" t="str">
         <f t="shared" ref="O22" si="6">Q20</f>
         <v>82</v>
       </c>
-      <c r="P22" s="264" t="s">
+      <c r="P22" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q22" s="264" t="s">
+      <c r="Q22" s="192" t="s">
         <v>298</v>
       </c>
-      <c r="R22" s="262"/>
-      <c r="S22" s="263" t="s">
+      <c r="R22" s="190"/>
+      <c r="S22" s="191" t="s">
         <v>301</v>
       </c>
-      <c r="T22" s="274"/>
-      <c r="U22" s="285" t="s">
+      <c r="T22" s="273"/>
+      <c r="U22" s="278" t="s">
         <v>180</v>
       </c>
-      <c r="V22" s="260" t="s">
+      <c r="V22" s="188" t="s">
         <v>65</v>
       </c>
-      <c r="W22" s="188"/>
-      <c r="X22" s="251"/>
-      <c r="Y22" s="251"/>
-      <c r="Z22" s="251"/>
-      <c r="AA22" s="251"/>
-      <c r="AB22" s="251"/>
-      <c r="AC22" s="251"/>
-      <c r="AD22" s="251"/>
-      <c r="AE22" s="251"/>
-      <c r="AF22" s="252"/>
+      <c r="W22" s="232"/>
+      <c r="X22" s="255"/>
+      <c r="Y22" s="255"/>
+      <c r="Z22" s="255"/>
+      <c r="AA22" s="255"/>
+      <c r="AB22" s="255"/>
+      <c r="AC22" s="255"/>
+      <c r="AD22" s="255"/>
+      <c r="AE22" s="255"/>
+      <c r="AF22" s="256"/>
     </row>
     <row r="23" spans="2:32" ht="20" customHeight="1">
       <c r="B23" s="9">
@@ -6060,25 +6070,25 @@
       <c r="M23" s="63">
         <v>-0.4</v>
       </c>
-      <c r="N23" s="240"/>
-      <c r="O23" s="261"/>
-      <c r="P23" s="264"/>
-      <c r="Q23" s="264"/>
-      <c r="R23" s="262"/>
-      <c r="S23" s="263"/>
-      <c r="T23" s="273"/>
-      <c r="U23" s="286"/>
-      <c r="V23" s="277"/>
-      <c r="W23" s="189"/>
-      <c r="X23" s="255"/>
-      <c r="Y23" s="255"/>
-      <c r="Z23" s="255"/>
-      <c r="AA23" s="255"/>
-      <c r="AB23" s="255"/>
-      <c r="AC23" s="255"/>
-      <c r="AD23" s="255"/>
-      <c r="AE23" s="255"/>
-      <c r="AF23" s="256"/>
+      <c r="N23" s="244"/>
+      <c r="O23" s="189"/>
+      <c r="P23" s="192"/>
+      <c r="Q23" s="192"/>
+      <c r="R23" s="190"/>
+      <c r="S23" s="191"/>
+      <c r="T23" s="272"/>
+      <c r="U23" s="279"/>
+      <c r="V23" s="276"/>
+      <c r="W23" s="233"/>
+      <c r="X23" s="259"/>
+      <c r="Y23" s="259"/>
+      <c r="Z23" s="259"/>
+      <c r="AA23" s="259"/>
+      <c r="AB23" s="259"/>
+      <c r="AC23" s="259"/>
+      <c r="AD23" s="259"/>
+      <c r="AE23" s="259"/>
+      <c r="AF23" s="260"/>
     </row>
     <row r="24" spans="2:32" ht="20" customHeight="1">
       <c r="B24" s="9">
@@ -6105,38 +6115,38 @@
       <c r="M24" s="67">
         <v>-0.1</v>
       </c>
-      <c r="N24" s="240"/>
-      <c r="O24" s="260" t="str">
+      <c r="N24" s="244"/>
+      <c r="O24" s="188" t="str">
         <f t="shared" ref="O24" si="7">Q22</f>
         <v>40</v>
       </c>
-      <c r="P24" s="264" t="s">
+      <c r="P24" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q24" s="264" t="s">
+      <c r="Q24" s="192" t="s">
         <v>299</v>
       </c>
-      <c r="R24" s="262"/>
-      <c r="S24" s="263" t="s">
+      <c r="R24" s="190"/>
+      <c r="S24" s="191" t="s">
         <v>301</v>
       </c>
-      <c r="T24" s="274"/>
-      <c r="U24" s="285" t="s">
+      <c r="T24" s="273"/>
+      <c r="U24" s="278" t="s">
         <v>181</v>
       </c>
-      <c r="V24" s="260" t="s">
+      <c r="V24" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="W24" s="188"/>
-      <c r="X24" s="251"/>
-      <c r="Y24" s="251"/>
-      <c r="Z24" s="251"/>
-      <c r="AA24" s="251"/>
-      <c r="AB24" s="251"/>
-      <c r="AC24" s="251"/>
-      <c r="AD24" s="251"/>
-      <c r="AE24" s="251"/>
-      <c r="AF24" s="252"/>
+      <c r="W24" s="232"/>
+      <c r="X24" s="255"/>
+      <c r="Y24" s="255"/>
+      <c r="Z24" s="255"/>
+      <c r="AA24" s="255"/>
+      <c r="AB24" s="255"/>
+      <c r="AC24" s="255"/>
+      <c r="AD24" s="255"/>
+      <c r="AE24" s="255"/>
+      <c r="AF24" s="256"/>
     </row>
     <row r="25" spans="2:32" ht="20" customHeight="1">
       <c r="B25" s="9"/>
@@ -6153,25 +6163,25 @@
       <c r="K25" s="10"/>
       <c r="L25" s="72"/>
       <c r="M25" s="63"/>
-      <c r="N25" s="240"/>
-      <c r="O25" s="261"/>
-      <c r="P25" s="264"/>
-      <c r="Q25" s="264"/>
-      <c r="R25" s="262"/>
-      <c r="S25" s="263"/>
-      <c r="T25" s="274"/>
-      <c r="U25" s="286"/>
-      <c r="V25" s="277"/>
-      <c r="W25" s="189"/>
-      <c r="X25" s="255"/>
-      <c r="Y25" s="255"/>
-      <c r="Z25" s="255"/>
-      <c r="AA25" s="255"/>
-      <c r="AB25" s="255"/>
-      <c r="AC25" s="255"/>
-      <c r="AD25" s="255"/>
-      <c r="AE25" s="255"/>
-      <c r="AF25" s="256"/>
+      <c r="N25" s="244"/>
+      <c r="O25" s="189"/>
+      <c r="P25" s="192"/>
+      <c r="Q25" s="192"/>
+      <c r="R25" s="190"/>
+      <c r="S25" s="191"/>
+      <c r="T25" s="273"/>
+      <c r="U25" s="279"/>
+      <c r="V25" s="276"/>
+      <c r="W25" s="233"/>
+      <c r="X25" s="259"/>
+      <c r="Y25" s="259"/>
+      <c r="Z25" s="259"/>
+      <c r="AA25" s="259"/>
+      <c r="AB25" s="259"/>
+      <c r="AC25" s="259"/>
+      <c r="AD25" s="259"/>
+      <c r="AE25" s="259"/>
+      <c r="AF25" s="260"/>
     </row>
     <row r="26" spans="2:32" ht="20" customHeight="1">
       <c r="B26" s="9"/>
@@ -6188,38 +6198,38 @@
       <c r="K26" s="10"/>
       <c r="L26" s="71"/>
       <c r="M26" s="68"/>
-      <c r="N26" s="240"/>
-      <c r="O26" s="260" t="str">
+      <c r="N26" s="244"/>
+      <c r="O26" s="188" t="str">
         <f t="shared" ref="O26" si="8">Q24</f>
         <v>20</v>
       </c>
-      <c r="P26" s="213" t="s">
+      <c r="P26" s="291" t="s">
         <v>22</v>
       </c>
-      <c r="Q26" s="213" t="s">
+      <c r="Q26" s="291" t="s">
         <v>300</v>
       </c>
       <c r="R26" s="283"/>
-      <c r="S26" s="279" t="s">
+      <c r="S26" s="299" t="s">
         <v>301</v>
       </c>
-      <c r="T26" s="272"/>
+      <c r="T26" s="271"/>
       <c r="U26" s="283" t="s">
         <v>181</v>
       </c>
       <c r="V26" s="280" t="s">
         <v>63</v>
       </c>
-      <c r="W26" s="188"/>
-      <c r="X26" s="251"/>
-      <c r="Y26" s="251"/>
-      <c r="Z26" s="251"/>
-      <c r="AA26" s="251"/>
-      <c r="AB26" s="251"/>
-      <c r="AC26" s="251"/>
-      <c r="AD26" s="251"/>
-      <c r="AE26" s="251"/>
-      <c r="AF26" s="252"/>
+      <c r="W26" s="232"/>
+      <c r="X26" s="255"/>
+      <c r="Y26" s="255"/>
+      <c r="Z26" s="255"/>
+      <c r="AA26" s="255"/>
+      <c r="AB26" s="255"/>
+      <c r="AC26" s="255"/>
+      <c r="AD26" s="255"/>
+      <c r="AE26" s="255"/>
+      <c r="AF26" s="256"/>
     </row>
     <row r="27" spans="2:32" ht="20" customHeight="1">
       <c r="B27" s="9"/>
@@ -6236,25 +6246,25 @@
       <c r="K27" s="10"/>
       <c r="L27" s="72"/>
       <c r="M27" s="65"/>
-      <c r="N27" s="240"/>
-      <c r="O27" s="261"/>
-      <c r="P27" s="213"/>
-      <c r="Q27" s="213"/>
+      <c r="N27" s="244"/>
+      <c r="O27" s="189"/>
+      <c r="P27" s="291"/>
+      <c r="Q27" s="291"/>
       <c r="R27" s="283"/>
-      <c r="S27" s="279"/>
-      <c r="T27" s="273"/>
+      <c r="S27" s="299"/>
+      <c r="T27" s="272"/>
       <c r="U27" s="284"/>
       <c r="V27" s="282"/>
-      <c r="W27" s="189"/>
-      <c r="X27" s="255"/>
-      <c r="Y27" s="255"/>
-      <c r="Z27" s="255"/>
-      <c r="AA27" s="255"/>
-      <c r="AB27" s="255"/>
-      <c r="AC27" s="255"/>
-      <c r="AD27" s="255"/>
-      <c r="AE27" s="255"/>
-      <c r="AF27" s="256"/>
+      <c r="W27" s="233"/>
+      <c r="X27" s="259"/>
+      <c r="Y27" s="259"/>
+      <c r="Z27" s="259"/>
+      <c r="AA27" s="259"/>
+      <c r="AB27" s="259"/>
+      <c r="AC27" s="259"/>
+      <c r="AD27" s="259"/>
+      <c r="AE27" s="259"/>
+      <c r="AF27" s="260"/>
     </row>
     <row r="28" spans="2:32" ht="20" customHeight="1">
       <c r="B28" s="9"/>
@@ -6271,27 +6281,27 @@
       <c r="K28" s="10"/>
       <c r="L28" s="71"/>
       <c r="M28" s="68"/>
-      <c r="N28" s="240"/>
-      <c r="O28" s="295"/>
-      <c r="P28" s="213" t="s">
+      <c r="N28" s="244"/>
+      <c r="O28" s="294"/>
+      <c r="P28" s="291" t="s">
         <v>22</v>
       </c>
-      <c r="Q28" s="213"/>
+      <c r="Q28" s="291"/>
       <c r="R28" s="283"/>
-      <c r="S28" s="279"/>
-      <c r="T28" s="272"/>
+      <c r="S28" s="299"/>
+      <c r="T28" s="271"/>
       <c r="U28" s="283"/>
       <c r="V28" s="280"/>
-      <c r="W28" s="188"/>
-      <c r="X28" s="251"/>
-      <c r="Y28" s="251"/>
-      <c r="Z28" s="251"/>
-      <c r="AA28" s="251"/>
-      <c r="AB28" s="251"/>
-      <c r="AC28" s="251"/>
-      <c r="AD28" s="251"/>
-      <c r="AE28" s="251"/>
-      <c r="AF28" s="252"/>
+      <c r="W28" s="232"/>
+      <c r="X28" s="255"/>
+      <c r="Y28" s="255"/>
+      <c r="Z28" s="255"/>
+      <c r="AA28" s="255"/>
+      <c r="AB28" s="255"/>
+      <c r="AC28" s="255"/>
+      <c r="AD28" s="255"/>
+      <c r="AE28" s="255"/>
+      <c r="AF28" s="256"/>
     </row>
     <row r="29" spans="2:32" ht="20" customHeight="1">
       <c r="B29" s="9"/>
@@ -6308,25 +6318,25 @@
       <c r="K29" s="10"/>
       <c r="L29" s="72"/>
       <c r="M29" s="65"/>
-      <c r="N29" s="240"/>
-      <c r="O29" s="299"/>
-      <c r="P29" s="213"/>
-      <c r="Q29" s="213"/>
+      <c r="N29" s="244"/>
+      <c r="O29" s="298"/>
+      <c r="P29" s="291"/>
+      <c r="Q29" s="291"/>
       <c r="R29" s="283"/>
-      <c r="S29" s="279"/>
-      <c r="T29" s="273"/>
+      <c r="S29" s="299"/>
+      <c r="T29" s="272"/>
       <c r="U29" s="284"/>
       <c r="V29" s="282"/>
-      <c r="W29" s="189"/>
-      <c r="X29" s="255"/>
-      <c r="Y29" s="255"/>
-      <c r="Z29" s="255"/>
-      <c r="AA29" s="255"/>
-      <c r="AB29" s="255"/>
-      <c r="AC29" s="255"/>
-      <c r="AD29" s="255"/>
-      <c r="AE29" s="255"/>
-      <c r="AF29" s="256"/>
+      <c r="W29" s="233"/>
+      <c r="X29" s="259"/>
+      <c r="Y29" s="259"/>
+      <c r="Z29" s="259"/>
+      <c r="AA29" s="259"/>
+      <c r="AB29" s="259"/>
+      <c r="AC29" s="259"/>
+      <c r="AD29" s="259"/>
+      <c r="AE29" s="259"/>
+      <c r="AF29" s="260"/>
     </row>
     <row r="30" spans="2:32" ht="20" customHeight="1">
       <c r="B30" s="9"/>
@@ -6343,27 +6353,27 @@
       <c r="K30" s="10"/>
       <c r="L30" s="71"/>
       <c r="M30" s="68"/>
-      <c r="N30" s="240"/>
-      <c r="O30" s="295"/>
-      <c r="P30" s="264" t="s">
+      <c r="N30" s="244"/>
+      <c r="O30" s="294"/>
+      <c r="P30" s="192" t="s">
         <v>22</v>
       </c>
-      <c r="Q30" s="264"/>
-      <c r="R30" s="262"/>
-      <c r="S30" s="263"/>
-      <c r="T30" s="272"/>
-      <c r="U30" s="289"/>
-      <c r="V30" s="291"/>
-      <c r="W30" s="257"/>
-      <c r="X30" s="251"/>
-      <c r="Y30" s="251"/>
-      <c r="Z30" s="251"/>
-      <c r="AA30" s="251"/>
-      <c r="AB30" s="251"/>
-      <c r="AC30" s="251"/>
-      <c r="AD30" s="251"/>
-      <c r="AE30" s="251"/>
-      <c r="AF30" s="252"/>
+      <c r="Q30" s="192"/>
+      <c r="R30" s="190"/>
+      <c r="S30" s="191"/>
+      <c r="T30" s="271"/>
+      <c r="U30" s="287"/>
+      <c r="V30" s="289"/>
+      <c r="W30" s="261"/>
+      <c r="X30" s="255"/>
+      <c r="Y30" s="255"/>
+      <c r="Z30" s="255"/>
+      <c r="AA30" s="255"/>
+      <c r="AB30" s="255"/>
+      <c r="AC30" s="255"/>
+      <c r="AD30" s="255"/>
+      <c r="AE30" s="255"/>
+      <c r="AF30" s="256"/>
     </row>
     <row r="31" spans="2:32" ht="20" customHeight="1">
       <c r="B31" s="9"/>
@@ -6380,25 +6390,25 @@
       <c r="K31" s="10"/>
       <c r="L31" s="71"/>
       <c r="M31" s="65"/>
-      <c r="N31" s="240"/>
-      <c r="O31" s="299"/>
-      <c r="P31" s="213"/>
-      <c r="Q31" s="213"/>
-      <c r="R31" s="262"/>
-      <c r="S31" s="263"/>
-      <c r="T31" s="273"/>
-      <c r="U31" s="290"/>
-      <c r="V31" s="292"/>
-      <c r="W31" s="259"/>
-      <c r="X31" s="255"/>
-      <c r="Y31" s="255"/>
-      <c r="Z31" s="255"/>
-      <c r="AA31" s="255"/>
-      <c r="AB31" s="255"/>
-      <c r="AC31" s="255"/>
-      <c r="AD31" s="255"/>
-      <c r="AE31" s="255"/>
-      <c r="AF31" s="256"/>
+      <c r="N31" s="244"/>
+      <c r="O31" s="298"/>
+      <c r="P31" s="291"/>
+      <c r="Q31" s="291"/>
+      <c r="R31" s="190"/>
+      <c r="S31" s="191"/>
+      <c r="T31" s="272"/>
+      <c r="U31" s="288"/>
+      <c r="V31" s="290"/>
+      <c r="W31" s="263"/>
+      <c r="X31" s="259"/>
+      <c r="Y31" s="259"/>
+      <c r="Z31" s="259"/>
+      <c r="AA31" s="259"/>
+      <c r="AB31" s="259"/>
+      <c r="AC31" s="259"/>
+      <c r="AD31" s="259"/>
+      <c r="AE31" s="259"/>
+      <c r="AF31" s="260"/>
     </row>
     <row r="32" spans="2:32" ht="20" customHeight="1" thickBot="1">
       <c r="B32" s="12"/>
@@ -6415,27 +6425,27 @@
       <c r="K32" s="11"/>
       <c r="L32" s="71"/>
       <c r="M32" s="68"/>
-      <c r="N32" s="240"/>
-      <c r="O32" s="295"/>
-      <c r="P32" s="293" t="s">
+      <c r="N32" s="244"/>
+      <c r="O32" s="294"/>
+      <c r="P32" s="292" t="s">
         <v>22</v>
       </c>
-      <c r="Q32" s="293"/>
-      <c r="R32" s="297"/>
-      <c r="S32" s="298"/>
-      <c r="T32" s="272"/>
+      <c r="Q32" s="292"/>
+      <c r="R32" s="296"/>
+      <c r="S32" s="297"/>
+      <c r="T32" s="271"/>
       <c r="U32" s="283"/>
       <c r="V32" s="280"/>
-      <c r="W32" s="257"/>
-      <c r="X32" s="251"/>
-      <c r="Y32" s="251"/>
-      <c r="Z32" s="251"/>
-      <c r="AA32" s="251"/>
-      <c r="AB32" s="251"/>
-      <c r="AC32" s="251"/>
-      <c r="AD32" s="251"/>
-      <c r="AE32" s="251"/>
-      <c r="AF32" s="252"/>
+      <c r="W32" s="261"/>
+      <c r="X32" s="255"/>
+      <c r="Y32" s="255"/>
+      <c r="Z32" s="255"/>
+      <c r="AA32" s="255"/>
+      <c r="AB32" s="255"/>
+      <c r="AC32" s="255"/>
+      <c r="AD32" s="255"/>
+      <c r="AE32" s="255"/>
+      <c r="AF32" s="256"/>
     </row>
     <row r="33" spans="2:32" ht="20" customHeight="1" thickTop="1" thickBot="1">
       <c r="B33" s="17"/>
@@ -6452,25 +6462,25 @@
       <c r="K33" s="15"/>
       <c r="L33" s="73"/>
       <c r="M33" s="69"/>
-      <c r="N33" s="241"/>
-      <c r="O33" s="296"/>
-      <c r="P33" s="294"/>
-      <c r="Q33" s="294"/>
-      <c r="R33" s="297"/>
-      <c r="S33" s="298"/>
-      <c r="T33" s="288"/>
-      <c r="U33" s="287"/>
+      <c r="N33" s="245"/>
+      <c r="O33" s="295"/>
+      <c r="P33" s="293"/>
+      <c r="Q33" s="293"/>
+      <c r="R33" s="296"/>
+      <c r="S33" s="297"/>
+      <c r="T33" s="286"/>
+      <c r="U33" s="285"/>
       <c r="V33" s="281"/>
-      <c r="W33" s="258"/>
-      <c r="X33" s="253"/>
-      <c r="Y33" s="253"/>
-      <c r="Z33" s="253"/>
-      <c r="AA33" s="253"/>
-      <c r="AB33" s="253"/>
-      <c r="AC33" s="253"/>
-      <c r="AD33" s="253"/>
-      <c r="AE33" s="253"/>
-      <c r="AF33" s="254"/>
+      <c r="W33" s="262"/>
+      <c r="X33" s="257"/>
+      <c r="Y33" s="257"/>
+      <c r="Z33" s="257"/>
+      <c r="AA33" s="257"/>
+      <c r="AB33" s="257"/>
+      <c r="AC33" s="257"/>
+      <c r="AD33" s="257"/>
+      <c r="AE33" s="257"/>
+      <c r="AF33" s="258"/>
     </row>
     <row r="34" spans="2:32" ht="14" thickTop="1">
       <c r="P34" s="28"/>
@@ -6532,6 +6542,7 @@
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="R26:R27"/>
     <mergeCell ref="S26:S27"/>
+    <mergeCell ref="P28:P29"/>
     <mergeCell ref="R14:R15"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="V32:V33"/>
@@ -6555,6 +6566,7 @@
     <mergeCell ref="V18:V19"/>
     <mergeCell ref="V16:V17"/>
     <mergeCell ref="U14:U15"/>
+    <mergeCell ref="T28:T29"/>
     <mergeCell ref="X10:AF11"/>
     <mergeCell ref="V14:V15"/>
     <mergeCell ref="V12:V13"/>
@@ -6568,7 +6580,6 @@
     <mergeCell ref="W18:W19"/>
     <mergeCell ref="W16:W17"/>
     <mergeCell ref="U12:U13"/>
-    <mergeCell ref="T28:T29"/>
     <mergeCell ref="T26:T27"/>
     <mergeCell ref="T24:T25"/>
     <mergeCell ref="T22:T23"/>
@@ -6603,7 +6614,6 @@
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="R12:R13"/>
     <mergeCell ref="S12:S13"/>
-    <mergeCell ref="P28:P29"/>
     <mergeCell ref="W1:AF1"/>
     <mergeCell ref="W2:AF6"/>
     <mergeCell ref="B5:F5"/>
@@ -6655,7 +6665,7 @@
   <phoneticPr fontId="28" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup scale="73" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="69" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -7997,7 +8007,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="20">
+    <row r="22" spans="1:11" ht="21">
       <c r="A22" s="469" t="s">
         <v>44</v>
       </c>
@@ -8025,7 +8035,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="21" thickBot="1">
+    <row r="23" spans="1:11" ht="22" thickBot="1">
       <c r="A23" s="469" t="s">
         <v>45</v>
       </c>
@@ -8072,7 +8082,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20">
+    <row r="25" spans="1:11" ht="21">
       <c r="A25" s="469" t="s">
         <v>49</v>
       </c>
@@ -8085,7 +8095,7 @@
       </c>
       <c r="E25" s="162"/>
     </row>
-    <row r="26" spans="1:11" ht="21" thickBot="1">
+    <row r="26" spans="1:11" ht="22" thickBot="1">
       <c r="A26" s="480" t="s">
         <v>50</v>
       </c>

</xml_diff>